<commit_message>
Mise à jour de plusieurs fonctions de FILINO le 02/02/2024
</commit_message>
<xml_diff>
--- a/RFILES/FILINO_15_10_VideosDemoProcess.xlsx
+++ b/RFILES/FILINO_15_10_VideosDemoProcess.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\R-4.3.1\Cerema\FILINO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\R-4.3.1\Cerema\FILINO\filino\RFILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1AFC9D-032F-41ED-8774-D77A17CEA81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF88994D-3B20-42D1-A666-B30F53668B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B16F40B-93F5-4251-9A18-8BD4D7492797}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$K$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$J$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="108">
   <si>
     <t>FILINO_MeP</t>
   </si>
@@ -219,9 +219,6 @@
     <t>FILINO_LAZ.qgs</t>
   </si>
   <si>
-    <t>VideoImageParSeconde</t>
-  </si>
-  <si>
     <t>LidarHD IGN - Classification</t>
   </si>
   <si>
@@ -337,6 +334,33 @@
   </si>
   <si>
     <t>FILINO_Cuvettes.qgs</t>
+  </si>
+  <si>
+    <t>Vert (&lt;50cm), Orange (50cm-1m), 1er Magenta (1 à 2m)…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file.path(dsnlayer,NomDirDIFF) </t>
+  </si>
+  <si>
+    <t>Végétation plus basse que le MNT Tin FILINO</t>
+  </si>
+  <si>
+    <t>Vert (&lt;50cm), Orange (50cm-1m), 1er Magenta (1 à 2m)…  (attention aux pentes fortes)</t>
+  </si>
+  <si>
+    <t>Différences entre le MNT TIN FILINO et Direct (sans FILINO)</t>
+  </si>
+  <si>
+    <t>Rouge négatif/Bordeaux positif pas 0.2, 0.5, 1, 2, 5m</t>
+  </si>
+  <si>
+    <t>_TIN_Filino_moins_VEGE_min_.gpkg$</t>
+  </si>
+  <si>
+    <t>_TIN_Filino_moins_TIN_Direct_.gpkg$</t>
+  </si>
+  <si>
+    <t>FILINO_RastDiff.qgs</t>
   </si>
 </sst>
 </file>
@@ -366,7 +390,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -389,17 +413,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -408,7 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E364DB-E3CC-47C1-9262-7D69928A3682}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C2" sqref="C2:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,18 +748,17 @@
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="63.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="133" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="133" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>67</v>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
@@ -758,29 +770,26 @@
         <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -792,24 +801,21 @@
       <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -821,26 +827,23 @@
       <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="H3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -852,28 +855,25 @@
       <c r="D4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="H4" s="1" t="s">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -885,30 +885,27 @@
       <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1">
-        <v>1</v>
+      <c r="E5" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>86</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -920,30 +917,27 @@
       <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1">
-        <v>1</v>
+      <c r="E6" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -955,30 +949,27 @@
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="1">
-        <v>1</v>
+      <c r="E7" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1">
@@ -990,30 +981,27 @@
       <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="1">
-        <v>1</v>
+      <c r="E8" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1">
@@ -1025,30 +1013,27 @@
       <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
+      <c r="E9" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K9" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1">
@@ -1060,30 +1045,27 @@
       <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="1">
-        <v>1</v>
+      <c r="E10" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K10" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1">
@@ -1095,30 +1077,27 @@
       <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="1">
-        <v>1</v>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1">
@@ -1130,30 +1109,27 @@
       <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="1">
-        <v>1</v>
+      <c r="E12" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1">
@@ -1165,30 +1141,27 @@
       <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="1">
-        <v>1</v>
+      <c r="E13" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1">
@@ -1200,30 +1173,27 @@
       <c r="D14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="1">
-        <v>1</v>
+      <c r="E14" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1">
@@ -1235,65 +1205,59 @@
       <c r="D15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="1">
-        <v>1</v>
+      <c r="E15" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>120</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" s="1" t="s">
+      <c r="F16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>120</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1">
@@ -1305,26 +1269,23 @@
       <c r="D17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="H17" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1">
@@ -1336,30 +1297,27 @@
       <c r="D18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="1">
-        <v>1</v>
+      <c r="E18" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1">
@@ -1371,30 +1329,27 @@
       <c r="D19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="1">
-        <v>1</v>
+      <c r="E19" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1">
@@ -1406,30 +1361,27 @@
       <c r="D20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="1">
-        <v>1</v>
+      <c r="E20" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1">
@@ -1441,30 +1393,27 @@
       <c r="D21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="1">
-        <v>1</v>
+      <c r="E21" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1">
@@ -1476,28 +1425,25 @@
       <c r="D22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="H22" s="1" t="s">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1">
@@ -1509,26 +1455,23 @@
       <c r="D23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="H23" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1">
@@ -1540,30 +1483,27 @@
       <c r="D24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="1">
-        <v>1</v>
+      <c r="E24" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>91</v>
+        <v>9</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K24" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1">
@@ -1575,30 +1515,27 @@
       <c r="D25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="1">
-        <v>1</v>
+      <c r="E25" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K25" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1">
@@ -1610,26 +1547,23 @@
       <c r="D26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="H26" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1">
@@ -1641,30 +1575,27 @@
       <c r="D27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="1">
-        <v>1</v>
+      <c r="E27" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1">
@@ -1676,30 +1607,27 @@
       <c r="D28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="1">
-        <v>1</v>
+      <c r="E28" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1">
@@ -1711,30 +1639,27 @@
       <c r="D29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="1">
-        <v>1</v>
+      <c r="E29" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>30</v>
       </c>
       <c r="B30" s="1">
@@ -1746,30 +1671,27 @@
       <c r="D30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="1">
-        <v>1</v>
+      <c r="E30" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>31</v>
       </c>
       <c r="B31" s="1">
@@ -1781,30 +1703,91 @@
       <c r="D31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="1">
-        <v>1</v>
+      <c r="E31" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>66</v>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1">
+        <v>120</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K29" xr:uid="{05E364DB-E3CC-47C1-9262-7D69928A3682}"/>
+  <autoFilter ref="A1:J29" xr:uid="{05E364DB-E3CC-47C1-9262-7D69928A3682}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>